<commit_message>
Finished the Sanity Filter and cleaned up the code slightly. Still need to clean up the code more and add comments where I can. Also need to create the method to easily get the stuff the UI needs and the way to output to a file when called from the UI.
</commit_message>
<xml_diff>
--- a/workbooks/CommsDatabase2.xlsx
+++ b/workbooks/CommsDatabase2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peter\Documents\NetBeansProjects\DisasterResponseTradeStudy\workbooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peter\Dropbox\PMASE - Capstone\Solution Design\Tech Matrices\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="46">
   <si>
     <t>ID</t>
   </si>
@@ -347,15 +347,15 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -680,7 +680,7 @@
   <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -692,7 +692,7 @@
     <col min="5" max="5" width="16.28515625" style="16" customWidth="1"/>
     <col min="6" max="9" width="9.140625" style="17"/>
     <col min="10" max="10" width="9.140625" style="18"/>
-    <col min="11" max="11" width="4.7109375" style="23" customWidth="1"/>
+    <col min="11" max="11" width="4.7109375" style="22" customWidth="1"/>
     <col min="12" max="13" width="12.7109375" style="20" customWidth="1"/>
   </cols>
   <sheetData>
@@ -727,7 +727,7 @@
       <c r="J1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="22" t="s">
+      <c r="K1" s="25" t="s">
         <v>45</v>
       </c>
       <c r="L1" s="9" t="s">
@@ -764,7 +764,7 @@
         <v>6</v>
       </c>
       <c r="J2" s="11"/>
-      <c r="K2" s="22"/>
+      <c r="K2" s="25"/>
       <c r="L2" s="12">
         <v>8</v>
       </c>
@@ -799,7 +799,7 @@
         <v>6</v>
       </c>
       <c r="J3" s="11"/>
-      <c r="K3" s="22"/>
+      <c r="K3" s="25"/>
       <c r="L3" s="12">
         <v>8000</v>
       </c>
@@ -836,7 +836,7 @@
       <c r="J4" s="11">
         <v>4</v>
       </c>
-      <c r="K4" s="22"/>
+      <c r="K4" s="25"/>
       <c r="L4" s="12">
         <v>8000</v>
       </c>
@@ -873,7 +873,7 @@
       <c r="J5" s="11">
         <v>4</v>
       </c>
-      <c r="K5" s="22"/>
+      <c r="K5" s="25"/>
       <c r="L5" s="12">
         <v>5</v>
       </c>
@@ -910,7 +910,7 @@
       <c r="J6" s="11">
         <v>4</v>
       </c>
-      <c r="K6" s="22"/>
+      <c r="K6" s="25"/>
       <c r="L6" s="12">
         <v>70</v>
       </c>
@@ -943,7 +943,7 @@
         <v>28</v>
       </c>
       <c r="J7" s="11"/>
-      <c r="K7" s="22"/>
+      <c r="K7" s="25"/>
       <c r="L7" s="12">
         <v>160</v>
       </c>
@@ -974,7 +974,7 @@
       <c r="J8" s="11">
         <v>14</v>
       </c>
-      <c r="K8" s="22"/>
+      <c r="K8" s="25"/>
       <c r="L8" s="12">
         <v>8</v>
       </c>
@@ -1005,7 +1005,7 @@
       <c r="J9" s="11">
         <v>14</v>
       </c>
-      <c r="K9" s="22"/>
+      <c r="K9" s="25"/>
       <c r="L9" s="12">
         <v>8</v>
       </c>
@@ -1040,7 +1040,7 @@
       <c r="J10" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="K10" s="22"/>
+      <c r="K10" s="25"/>
       <c r="L10" s="12">
         <v>200</v>
       </c>
@@ -1049,29 +1049,29 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="K11" s="22"/>
+      <c r="K11" s="25"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="K12" s="22"/>
+      <c r="K12" s="25"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="K13" s="22"/>
+      <c r="K13" s="25"/>
       <c r="L13" s="19"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="K14" s="22"/>
+      <c r="K14" s="25"/>
       <c r="L14" s="19"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="K15" s="22"/>
+      <c r="K15" s="25"/>
       <c r="L15" s="19"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="K16" s="22"/>
+      <c r="K16" s="25"/>
       <c r="L16" s="19"/>
     </row>
     <row r="17" spans="11:12" x14ac:dyDescent="0.25">
-      <c r="K17" s="22"/>
+      <c r="K17" s="25"/>
       <c r="L17" s="19"/>
     </row>
     <row r="18" spans="11:12" x14ac:dyDescent="0.25">
@@ -1093,7 +1093,30 @@
   <mergeCells count="1">
     <mergeCell ref="K1:K17"/>
   </mergeCells>
+  <dataValidations count="3">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576 L1:L1048576 M1:M1048576">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="textLength" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1048576">
+      <formula1>0</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'Supported Data Type'!$E$2:$E$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2:C10</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1196,10 +1219,10 @@
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1207,36 +1230,61 @@
     <col min="1" max="1" width="27.42578125" style="15" customWidth="1"/>
     <col min="2" max="2" width="10.85546875" style="14" customWidth="1"/>
     <col min="3" max="3" width="17.28515625" style="15" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" style="14" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" style="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="25" t="s">
+      <c r="B1" s="23"/>
+      <c r="C1" s="24" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="23"/>
+      <c r="E1" s="24" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>36</v>
       </c>
       <c r="C2" s="15" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E2" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>37</v>
       </c>
       <c r="C3" s="15" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E3" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>38</v>
+      </c>
+      <c r="E4" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E5" s="15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E6" s="15">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added method for Mike
</commit_message>
<xml_diff>
--- a/workbooks/CommsDatabase2.xlsx
+++ b/workbooks/CommsDatabase2.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peter\Dropbox\PMASE - Capstone\Solution Design\Tech Matrices\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peter\Documents\NetBeansProjects\DisasterResponseTradeStudy\workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18750" windowHeight="12690"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18750" windowHeight="12690" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Communication" sheetId="2" r:id="rId1"/>
@@ -157,13 +157,13 @@
     <t>Sort Orders</t>
   </si>
   <si>
-    <t xml:space="preserve">Data Rate </t>
-  </si>
-  <si>
     <t>Mbps</t>
   </si>
   <si>
     <t>Custom Values After This Column</t>
+  </si>
+  <si>
+    <t>Data Rate</t>
   </si>
 </sst>
 </file>
@@ -679,8 +679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView topLeftCell="B1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -728,7 +728,7 @@
         <v>8</v>
       </c>
       <c r="K1" s="25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L1" s="9" t="s">
         <v>2</v>
@@ -1127,8 +1127,8 @@
   </sheetPr>
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1175,13 +1175,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B3" s="1">
         <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>38</v>

</xml_diff>

<commit_message>
Finished Outputer. Need to extract to interface still though to remain with pattern
</commit_message>
<xml_diff>
--- a/workbooks/CommsDatabase2.xlsx
+++ b/workbooks/CommsDatabase2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18750" windowHeight="12690" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18750" windowHeight="12690"/>
   </bookViews>
   <sheets>
     <sheet name="Communication" sheetId="2" r:id="rId1"/>
@@ -91,9 +91,6 @@
     <t>Hybrid Microwave</t>
   </si>
   <si>
-    <t>10,11,12,13,14,15</t>
-  </si>
-  <si>
     <t>PtP Microwave</t>
   </si>
   <si>
@@ -106,9 +103,6 @@
     <t>BLOS</t>
   </si>
   <si>
-    <t>1,2,3,4,5,6,7,8,9</t>
-  </si>
-  <si>
     <t>2,6,12</t>
   </si>
   <si>
@@ -164,6 +158,12 @@
   </si>
   <si>
     <t>Data Rate</t>
+  </si>
+  <si>
+    <t>9,10,11,12,13,14</t>
+  </si>
+  <si>
+    <t>1,2,3,4,5,6,7,8,9,14</t>
   </si>
 </sst>
 </file>
@@ -679,8 +679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -728,7 +728,7 @@
         <v>8</v>
       </c>
       <c r="K1" s="25" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="L1" s="9" t="s">
         <v>2</v>
@@ -868,7 +868,7 @@
         <v>19</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="J5" s="11">
         <v>4</v>
@@ -895,7 +895,7 @@
         <v>5</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="8">
@@ -905,7 +905,7 @@
         <v>19</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="J6" s="11">
         <v>4</v>
@@ -923,7 +923,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7" s="4">
         <v>4</v>
@@ -932,7 +932,7 @@
         <v>10</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
@@ -940,7 +940,7 @@
         <v>19</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="J7" s="11"/>
       <c r="K7" s="25"/>
@@ -956,7 +956,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8" s="4">
         <v>1</v>
@@ -987,7 +987,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9" s="4">
         <v>1</v>
@@ -1018,7 +1018,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10" s="4">
         <v>5</v>
@@ -1027,15 +1027,15 @@
         <v>70</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
       <c r="H10" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="J10" s="11" t="s">
         <v>9</v>
@@ -1097,7 +1097,7 @@
     <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576 L1:L1048576 M1:M1048576">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576 L1:M1048576">
       <formula1>0</formula1>
     </dataValidation>
     <dataValidation type="textLength" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1048576">
@@ -1127,7 +1127,7 @@
   </sheetPr>
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+    <sheetView zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1141,53 +1141,53 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="D1" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="E1" s="13" t="s">
         <v>31</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B2" s="1">
         <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B3" s="1">
         <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1236,11 +1236,11 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B1" s="23"/>
       <c r="C1" s="24" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D1" s="23"/>
       <c r="E1" s="24" t="s">
@@ -1249,10 +1249,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E2" s="15">
         <v>1</v>
@@ -1260,10 +1260,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E3" s="15">
         <v>2</v>
@@ -1271,7 +1271,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E4" s="15">
         <v>3</v>

</xml_diff>

<commit_message>
Addressing issue #21. Hope to have fixed it
</commit_message>
<xml_diff>
--- a/workbooks/CommsDatabase2.xlsx
+++ b/workbooks/CommsDatabase2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peter\Documents\NetBeansProjects\DisasterResponseTradeStudy\workbooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peter\Dropbox\PMASE - Capstone\Solution Design\Tech Matrices\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Custom Column Description" sheetId="3" r:id="rId2"/>
     <sheet name="Supported Data Type" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171026"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="48">
   <si>
     <t>ID</t>
   </si>
@@ -55,9 +55,6 @@
     <t>Disaster Effect</t>
   </si>
   <si>
-    <t>4,9</t>
-  </si>
-  <si>
     <t>Data Rate (Mbps)</t>
   </si>
   <si>
@@ -100,9 +97,6 @@
     <t>3G Cellular</t>
   </si>
   <si>
-    <t>BLOS</t>
-  </si>
-  <si>
     <t>2,6,12</t>
   </si>
   <si>
@@ -160,10 +154,22 @@
     <t>Data Rate</t>
   </si>
   <si>
-    <t>9,10,11,12,13,14</t>
-  </si>
-  <si>
-    <t>1,2,3,4,5,6,7,8,9,14</t>
+    <t>1,2,3,4,5,6,7,8,9,14,15</t>
+  </si>
+  <si>
+    <t>9,10,11,12,13,14,15</t>
+  </si>
+  <si>
+    <t>Troposcatter</t>
+  </si>
+  <si>
+    <t>HF</t>
+  </si>
+  <si>
+    <t>1,2</t>
+  </si>
+  <si>
+    <t>9,13</t>
   </si>
 </sst>
 </file>
@@ -288,7 +294,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -353,6 +359,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
@@ -679,8 +688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -689,7 +698,7 @@
     <col min="2" max="2" width="28.28515625" style="15" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" style="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="15"/>
-    <col min="5" max="5" width="16.28515625" style="16" customWidth="1"/>
+    <col min="5" max="5" width="21" style="16" bestFit="1" customWidth="1"/>
     <col min="6" max="9" width="9.140625" style="17"/>
     <col min="10" max="10" width="9.140625" style="18"/>
     <col min="11" max="11" width="4.7109375" style="22" customWidth="1"/>
@@ -707,10 +716,10 @@
         <v>3</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>4</v>
@@ -727,14 +736,14 @@
       <c r="J1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="25" t="s">
-        <v>42</v>
+      <c r="K1" s="26" t="s">
+        <v>40</v>
       </c>
       <c r="L1" s="9" t="s">
         <v>2</v>
       </c>
       <c r="M1" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -742,7 +751,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" s="4">
         <v>1</v>
@@ -751,20 +760,18 @@
         <v>2</v>
       </c>
       <c r="E2" s="6"/>
-      <c r="F2" s="8">
-        <v>13</v>
-      </c>
+      <c r="F2" s="8"/>
       <c r="G2" s="8">
         <v>13</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I2" s="8">
         <v>6</v>
       </c>
       <c r="J2" s="11"/>
-      <c r="K2" s="25"/>
+      <c r="K2" s="26"/>
       <c r="L2" s="12">
         <v>8</v>
       </c>
@@ -777,7 +784,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" s="4">
         <v>1</v>
@@ -786,7 +793,7 @@
         <v>2</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="8">
@@ -799,9 +806,9 @@
         <v>6</v>
       </c>
       <c r="J3" s="11"/>
-      <c r="K3" s="25"/>
+      <c r="K3" s="26"/>
       <c r="L3" s="12">
-        <v>8000</v>
+        <v>20000</v>
       </c>
       <c r="M3" s="12">
         <v>0.5</v>
@@ -812,7 +819,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" s="4">
         <v>2</v>
@@ -821,7 +828,7 @@
         <v>10</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F4" s="8"/>
       <c r="G4" s="8">
@@ -834,11 +841,11 @@
         <v>6</v>
       </c>
       <c r="J4" s="11">
-        <v>4</v>
-      </c>
-      <c r="K4" s="25"/>
+        <v>13</v>
+      </c>
+      <c r="K4" s="26"/>
       <c r="L4" s="12">
-        <v>8000</v>
+        <v>20000</v>
       </c>
       <c r="M4" s="12">
         <v>25</v>
@@ -849,7 +856,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" s="4">
         <v>2</v>
@@ -858,22 +865,20 @@
         <v>3</v>
       </c>
       <c r="E5" s="6"/>
-      <c r="F5" s="8">
-        <v>13</v>
-      </c>
+      <c r="F5" s="8"/>
       <c r="G5" s="8">
         <v>13</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J5" s="11">
-        <v>4</v>
-      </c>
-      <c r="K5" s="25"/>
+        <v>13</v>
+      </c>
+      <c r="K5" s="26"/>
       <c r="L5" s="12">
         <v>5</v>
       </c>
@@ -886,7 +891,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" s="4">
         <v>3</v>
@@ -895,22 +900,22 @@
         <v>5</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="8">
         <v>13</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J6" s="11">
-        <v>4</v>
-      </c>
-      <c r="K6" s="25"/>
+        <v>13</v>
+      </c>
+      <c r="K6" s="26"/>
       <c r="L6" s="12">
         <v>70</v>
       </c>
@@ -923,7 +928,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" s="4">
         <v>4</v>
@@ -932,18 +937,18 @@
         <v>10</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
       <c r="H7" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J7" s="11"/>
-      <c r="K7" s="25"/>
+      <c r="K7" s="26"/>
       <c r="L7" s="12">
         <v>160</v>
       </c>
@@ -956,7 +961,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C8" s="4">
         <v>1</v>
@@ -974,7 +979,7 @@
       <c r="J8" s="11">
         <v>14</v>
       </c>
-      <c r="K8" s="25"/>
+      <c r="K8" s="26"/>
       <c r="L8" s="12">
         <v>8</v>
       </c>
@@ -987,7 +992,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" s="4">
         <v>1</v>
@@ -1005,7 +1010,7 @@
       <c r="J9" s="11">
         <v>14</v>
       </c>
-      <c r="K9" s="25"/>
+      <c r="K9" s="26"/>
       <c r="L9" s="12">
         <v>8</v>
       </c>
@@ -1018,7 +1023,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="C10" s="4">
         <v>5</v>
@@ -1027,20 +1032,20 @@
         <v>70</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
       <c r="H10" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J10" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="K10" s="25"/>
+        <v>47</v>
+      </c>
+      <c r="K10" s="26"/>
       <c r="L10" s="12">
         <v>200</v>
       </c>
@@ -1049,29 +1054,56 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="K11" s="25"/>
+      <c r="A11" s="25">
+        <v>10</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="15">
+        <v>1</v>
+      </c>
+      <c r="D11" s="15">
+        <v>5</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="I11" s="8">
+        <v>6</v>
+      </c>
+      <c r="J11" s="11">
+        <v>13</v>
+      </c>
+      <c r="K11" s="26"/>
+      <c r="L11" s="20">
+        <v>20000</v>
+      </c>
+      <c r="M11" s="20">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="K12" s="25"/>
+      <c r="K12" s="26"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="K13" s="25"/>
+      <c r="K13" s="26"/>
       <c r="L13" s="19"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="K14" s="25"/>
+      <c r="K14" s="26"/>
       <c r="L14" s="19"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="K15" s="25"/>
+      <c r="K15" s="26"/>
       <c r="L15" s="19"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="K16" s="25"/>
+      <c r="K16" s="26"/>
       <c r="L16" s="19"/>
     </row>
     <row r="17" spans="11:12" x14ac:dyDescent="0.25">
-      <c r="K17" s="25"/>
+      <c r="K17" s="26"/>
       <c r="L17" s="19"/>
     </row>
     <row r="18" spans="11:12" x14ac:dyDescent="0.25">
@@ -1141,53 +1173,53 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="D1" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="E1" s="13" t="s">
         <v>29</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B2" s="1">
         <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B3" s="1">
         <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1236,11 +1268,11 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B1" s="23"/>
       <c r="C1" s="24" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D1" s="23"/>
       <c r="E1" s="24" t="s">
@@ -1249,10 +1281,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E2" s="15">
         <v>1</v>
@@ -1260,10 +1292,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E3" s="15">
         <v>2</v>
@@ -1271,7 +1303,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E4" s="15">
         <v>3</v>

</xml_diff>